<commit_message>
There is a problem when a user submits a job with a job name with a space in. I have created a quick fix but I need to remove that field from the squeue command. This requires me to update the entire script. I need a better way to index arrays which makes more sense.
</commit_message>
<xml_diff>
--- a/xlsx/time_stats_large_long_2025-03-25.xlsx
+++ b/xlsx/time_stats_large_long_2025-03-25.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B27"/>
+  <dimension ref="A1:B29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,39 +447,39 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>10080.46666666667</v>
+        <v>9016.033333333333</v>
       </c>
       <c r="B2" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>9016.033333333333</v>
+        <v>6299.216666666666</v>
       </c>
       <c r="B3" t="n">
-        <v>43200</v>
+        <v>10080</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>6299.216666666666</v>
+        <v>0</v>
       </c>
       <c r="B4" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>4514.683333333333</v>
+        <v>0</v>
       </c>
       <c r="B5" t="n">
-        <v>7200</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>1275.333333333333</v>
+        <v>5937.266666666666</v>
       </c>
       <c r="B6" t="n">
         <v>43200</v>
@@ -487,15 +487,15 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>149.2166666666667</v>
+        <v>5804.433333333333</v>
       </c>
       <c r="B7" t="n">
-        <v>2880</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>2495.85</v>
+        <v>5704.25</v>
       </c>
       <c r="B8" t="n">
         <v>43200</v>
@@ -503,7 +503,7 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>1784.75</v>
+        <v>1623.383333333333</v>
       </c>
       <c r="B9" t="n">
         <v>43200</v>
@@ -511,39 +511,39 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>1186.916666666667</v>
+        <v>1275.333333333333</v>
       </c>
       <c r="B10" t="n">
-        <v>2880</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>349.0166666666667</v>
+        <v>2495.85</v>
       </c>
       <c r="B11" t="n">
-        <v>2880</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>0.08333333333333333</v>
+        <v>1784.75</v>
       </c>
       <c r="B12" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>36.2</v>
+        <v>1186.916666666667</v>
       </c>
       <c r="B13" t="n">
-        <v>10080</v>
+        <v>2880</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>39.18333333333333</v>
+        <v>628.5666666666667</v>
       </c>
       <c r="B14" t="n">
         <v>10080</v>
@@ -551,23 +551,23 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>31.75</v>
+        <v>67.84999999999999</v>
       </c>
       <c r="B15" t="n">
-        <v>10080</v>
+        <v>20160</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>3.566666666666666</v>
+        <v>1117.783333333333</v>
       </c>
       <c r="B16" t="n">
-        <v>10080</v>
+        <v>20160</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>5.6</v>
+        <v>1024.983333333333</v>
       </c>
       <c r="B17" t="n">
         <v>10080</v>
@@ -575,7 +575,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>628.5666666666667</v>
+        <v>100.45</v>
       </c>
       <c r="B18" t="n">
         <v>10080</v>
@@ -583,39 +583,39 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>8.616666666666667</v>
+        <v>568.25</v>
       </c>
       <c r="B19" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>15.96666666666667</v>
+        <v>788.4</v>
       </c>
       <c r="B20" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>67.84999999999999</v>
+        <v>14.58333333333333</v>
       </c>
       <c r="B21" t="n">
-        <v>20160</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>100.45</v>
+        <v>13.26666666666667</v>
       </c>
       <c r="B22" t="n">
-        <v>10080</v>
+        <v>43200</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>568.25</v>
+        <v>138.05</v>
       </c>
       <c r="B23" t="n">
         <v>43200</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>788.4</v>
+        <v>107.0666666666667</v>
       </c>
       <c r="B24" t="n">
         <v>43200</v>
@@ -631,7 +631,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>14.58333333333333</v>
+        <v>25.98333333333333</v>
       </c>
       <c r="B25" t="n">
         <v>43200</v>
@@ -639,7 +639,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>13.26666666666667</v>
+        <v>5.15</v>
       </c>
       <c r="B26" t="n">
         <v>43200</v>
@@ -647,9 +647,25 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>138.05</v>
+        <v>0</v>
       </c>
       <c r="B27" t="n">
+        <v>43200</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>147.6</v>
+      </c>
+      <c r="B28" t="n">
+        <v>10080</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>0</v>
+      </c>
+      <c r="B29" t="n">
         <v>43200</v>
       </c>
     </row>

</xml_diff>